<commit_message>
Código para carregar planilha
</commit_message>
<xml_diff>
--- a/OpenReport.Tests/Resources/Modelo03.xlsx
+++ b/OpenReport.Tests/Resources/Modelo03.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\Tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\DotNet Core\OpenReport\OpenReport.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7210429-9DFA-40C7-9CFA-4DF1B6C8CBCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C5818F-A616-49C6-8687-6A87F8ECFB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C07BB88-E494-49D0-B9DA-A6627AFD668D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C07BB88-E494-49D0-B9DA-A6627AFD668D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
@@ -86,7 +88,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -193,13 +195,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -209,19 +215,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Moeda" xfId="3" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 6" xfId="1" xr:uid="{B61CBCC3-276B-4285-A019-6982B2C7E1A5}"/>
     <cellStyle name="Normal 8" xfId="2" xr:uid="{1FE6946B-27CC-47E5-A568-B74B5349927C}"/>
@@ -240,7 +242,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -550,18 +552,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="3" spans="1:3" ht="12" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
@@ -586,23 +588,23 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
@@ -622,21 +624,21 @@
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -649,4 +651,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF3117A-A959-4CBA-892C-1C50F9E7B125}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="9" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CB6B55-2335-4FBC-8CBE-CDC228A5DC14}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="9" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>